<commit_message>
Update PM03 TIdsregistrering for Rasmus.xlsx
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM03 TIdsregistrering for Rasmus.xlsx
+++ b/08 Project Management/Tidsregistrering/PM03 TIdsregistrering for Rasmus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasmu\Documents\GitHub\1AarsProjekt\08 Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61A72D8-D6E6-409E-8826-B627D1075705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC4ED07-4097-4092-8088-8E4EBDC4AA08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
+    <workbookView xWindow="3390" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Tidsregistrering af (Navn)</t>
   </si>
@@ -169,6 +169,21 @@
   </si>
   <si>
     <t>Use-case diagram</t>
+  </si>
+  <si>
+    <t>Furps+</t>
+  </si>
+  <si>
+    <t>review af MockUp</t>
+  </si>
+  <si>
+    <t>Risikoanalyse</t>
+  </si>
+  <si>
+    <t>Review af Metrikker</t>
+  </si>
+  <si>
+    <t>Fællesgennemgang af projektplan</t>
   </si>
 </sst>
 </file>
@@ -751,7 +766,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,73 +891,118 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+      <c r="A6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="15">
+        <v>43963</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.375</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.4375</v>
+      </c>
       <c r="F6" s="21"/>
       <c r="G6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H6" s="1">
         <f>SUM(G$3:G6)</f>
-        <v>0.19444444444444436</v>
+        <v>0.25694444444444436</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="A7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="15">
+        <v>43963</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.4375</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="F7" s="21"/>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333315E-2</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(G$3:G7)</f>
-        <v>0.19444444444444436</v>
+        <v>0.27777777777777768</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="A8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="15">
+        <v>43963</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.12500000000000006</v>
       </c>
       <c r="H8" s="1">
         <f>SUM(G$3:G8)</f>
-        <v>0.19444444444444436</v>
+        <v>0.40277777777777773</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="A9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="15">
+        <v>43963</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="F9" s="21"/>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333259E-2</v>
       </c>
       <c r="H9" s="1">
         <f>SUM(G$3:G9)</f>
-        <v>0.19444444444444436</v>
+        <v>0.42361111111111099</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="A10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="15">
+        <v>43963</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0.6875</v>
+      </c>
       <c r="F10" s="21"/>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="H10" s="1">
         <f>SUM(G$3:G10)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -956,7 +1016,7 @@
       </c>
       <c r="H11" s="1">
         <f>SUM(G$3:G11)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -970,7 +1030,7 @@
       </c>
       <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -984,7 +1044,7 @@
       </c>
       <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -996,7 +1056,7 @@
       </c>
       <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1008,7 +1068,7 @@
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1020,7 +1080,7 @@
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1032,7 +1092,7 @@
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1044,7 +1104,7 @@
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1056,7 +1116,7 @@
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1068,7 +1128,7 @@
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1080,7 +1140,7 @@
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1092,7 +1152,7 @@
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1104,7 +1164,7 @@
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1116,7 +1176,7 @@
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1127,7 +1187,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1138,7 +1198,7 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1149,7 +1209,7 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1160,7 +1220,7 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1171,7 +1231,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1182,7 +1242,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1193,7 +1253,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1204,7 +1264,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>0.19444444444444436</v>
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>